<commit_message>
Update as per word format
</commit_message>
<xml_diff>
--- a/data/master_data.xlsx
+++ b/data/master_data.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hp\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B958AB94-2563-4B40-8C27-DB833A2465BA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AF2F94B-FE3E-4B9B-BDB8-470C7EB06A5C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8364" activeTab="2" xr2:uid="{C736D8F4-95B0-4C8A-84B8-49E1B3723E1A}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8364" activeTab="3" xr2:uid="{C736D8F4-95B0-4C8A-84B8-49E1B3723E1A}"/>
   </bookViews>
   <sheets>
     <sheet name="Region Mapping" sheetId="5" r:id="rId1"/>
     <sheet name="NPI Sheet" sheetId="4" r:id="rId2"/>
     <sheet name="Product List" sheetId="3" r:id="rId3"/>
+    <sheet name="Activity List" sheetId="6" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Product List'!$A$1:$E$1</definedName>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="69">
   <si>
     <t>Product</t>
   </si>
@@ -216,6 +217,40 @@
   </si>
   <si>
     <t>Realised Value in Rs</t>
+  </si>
+  <si>
+    <t>Activity Type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">One To One Farmer Contacts </t>
+  </si>
+  <si>
+    <t>Phone Contacts by MIT Team</t>
+  </si>
+  <si>
+    <t>Village Meetings ( Group meetings )-MDOs</t>
+  </si>
+  <si>
+    <t>Spot 
+Demos</t>
+  </si>
+  <si>
+    <t>Field Days</t>
+  </si>
+  <si>
+    <t>Organized Farmer Meetings - MIEs</t>
+  </si>
+  <si>
+    <t>LPDs - MIEs</t>
+  </si>
+  <si>
+    <t>Harvest Days - MIEs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Branded Van Campaign ( BVC ) </t>
+  </si>
+  <si>
+    <t>Innovative Campaign</t>
   </si>
 </sst>
 </file>
@@ -705,7 +740,7 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView zoomScale="102" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -789,7 +824,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -979,8 +1014,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39B4F798-044A-4C5C-B5E4-F8454D2FCC44}">
   <dimension ref="A1:E38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -1645,4 +1680,77 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB9E9DEF-D5C7-42A0-8AB0-15E654D93369}">
+  <dimension ref="A1:A11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:A11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8"/>
+  <cols>
+    <col min="1" max="1" width="41.8984375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1">
+      <c r="A11" t="s">
+        <v>68</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>